<commit_message>
chore: update inventory report
</commit_message>
<xml_diff>
--- a/reports/2025/inventory_2025-08.xlsx
+++ b/reports/2025/inventory_2025-08.xlsx
@@ -626,12 +626,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P055</t>
+          <t>P-0155</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-936534850</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-797686298-salsa-para-alitas-sabor-mezcal-38l-inigualabe-e-innovadora-_JM#position=11&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -674,12 +674,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P080</t>
+          <t>P-0155</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.mercadolibre.com.mx/mr-wings-tamarindo-en-galon-38l/p/MLM16595091?pdp_filters=seller_id:206710930#searchVariation=MLM16595091&amp;position=2&amp;search_layout=stack&amp;type=product&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-893622220-salsa-sabor-mezcal-38lt-_JM#position=43&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -722,12 +722,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P093</t>
+          <t>P055</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-756586369-salsa-lemon-pepper-para-alitas-38-l-al-mejor-precio-_JM#position=7&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-936534850</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -770,12 +770,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P101</t>
+          <t>P069</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-755933726-salsa-ajo-parmesano-38-lts-para-alitas-al-mejor-precio-_JM#position=8&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-755923056-salsa-picante-buffalo-para-alitas-38-l-al-mejor-precio-_JM#position=18&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -818,12 +818,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P079</t>
+          <t>P069</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-770206770-salsa-bbq-barbecue-para-alitas-38-l-al-mejor-precio-_JM#position=9&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-825377787-salsa-bufalo-para-alitas-38-l-al-mejor-precio-_JM#position=12&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -866,12 +866,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P080</t>
+          <t>P070</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-756568095-salsa-tamarindo-para-alitas-38-l-al-mejor-precio-_JM#position=10&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-756574513-sazonador-cajun-en-polvo-bote-650g-al-mejor-precio-_JM#position=35&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -914,12 +914,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P-0155</t>
+          <t>P071</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-797686298-salsa-para-alitas-sabor-mezcal-38l-inigualabe-e-innovadora-_JM#position=11&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-756582654-salsa-picante-original-h-para-alitas-38-l-al-mejor-precio-_JM#position=19&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -962,12 +962,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P078</t>
+          <t>P073</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-756571227-salsa-teriyaki-para-alitas-38-l-al-mejor-precio-_JM#position=12&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-755952625-salsa-honey-mustard-mostaza-dulce-38-l-al-mejor-precio-_JM#position=14&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1010,12 +1010,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P073</t>
+          <t>P074</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-755952625-salsa-honey-mustard-mostaza-dulce-38-l-al-mejor-precio-_JM#position=14&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-874460232-salsa-para-alitas-crema-de-habanero-38lts-_JM#position=34&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1058,12 +1058,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P089</t>
+          <t>P075</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-756586580-sazonador-lemon-pepper-en-polvo-bote-800g-al-mejor-precio-_JM#position=16&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-755926452-salsa-picante-pina-hot-para-alitas-38-l-al-mejor-precio-_JM#position=19&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1106,12 +1106,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>P069</t>
+          <t>P075</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-755923056-salsa-picante-buffalo-para-alitas-38-l-al-mejor-precio-_JM#position=18&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-825295407-salsa-pina-hot-para-alitas-38-l-al-mejor-precio-_JM#position=4&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1154,12 +1154,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>P075</t>
+          <t>P076</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-755926452-salsa-picante-pina-hot-para-alitas-38-l-al-mejor-precio-_JM#position=19&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-755917563-salsa-picante-para-alitas-bbq-chipotle-38l-_JM#position=22&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1202,12 +1202,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>P086</t>
+          <t>P076</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-756582084-salsa-naranja-chipotle-para-alitas-38-l-al-mejor-precio-_JM#position=21&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-868471591-salsa-bbq-chipotle-_JM#position=25&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1250,12 +1250,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>P076</t>
+          <t>P077</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-755917563-salsa-picante-para-alitas-bbq-chipotle-38l-_JM#position=22&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-755923937-salsa-mango-habanero-para-alitas-38-l-al-mejor-precio-_JM#position=45&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1346,12 +1346,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>P083</t>
+          <t>P077</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-755921589-salsa-extra-hot-38l-salsa-extra-picante-para-alitas-_JM#position=26&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-874397634-salsa-mango-habanero-42kg-para-alitas-_JM#position=37&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1394,12 +1394,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>P081</t>
+          <t>P077</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-756571010-salsa-picante-bbq-barbecue-habanero-para-alitas-38-l-_JM#position=27&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904247331-salsa-para-alitas-mango-habanero-23-kg-_JM#position=31&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1442,12 +1442,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>P085</t>
+          <t>P078</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-756567270-salsa-picante-cajun-para-alitas-38-l-al-mejor-precio-_JM#position=28&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-756571227-salsa-teriyaki-para-alitas-38-l-al-mejor-precio-_JM#position=12&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1490,12 +1490,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>P137</t>
+          <t>P078</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-848013478-salsa-de-guacamole-para-alitas-38-l-al-mejor-precio-_JM#position=32&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-814451280-salsa-teriyaki-38-lts-para-alitas-al-mejor-precio-_JM#position=1&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1538,12 +1538,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>P084</t>
+          <t>P079</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-756567694-sazonador-fuego-en-polvo-bote-800g-al-mejor-precio-_JM#position=33&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-755920242-salsa-picante-bbq-barbecue-para-alitas-38-l-al-mejor-precio-_JM#position=48&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1586,12 +1586,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>P070</t>
+          <t>P079</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-756574513-sazonador-cajun-en-polvo-bote-650g-al-mejor-precio-_JM#position=35&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-770206770-salsa-bbq-barbecue-para-alitas-38-l-al-mejor-precio-_JM#position=9&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1634,12 +1634,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>P077</t>
+          <t>P079</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-755923937-salsa-mango-habanero-para-alitas-38-l-al-mejor-precio-_JM#position=45&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-788982442-salsa-bbq-barbecue-38l-para-alitas-mr-wings-al-mejor-precio-_JM#position=5&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1682,12 +1682,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>P079</t>
+          <t>P080</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-755920242-salsa-picante-bbq-barbecue-para-alitas-38-l-al-mejor-precio-_JM#position=48&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-756568095-salsa-tamarindo-para-alitas-38-l-al-mejor-precio-_JM#position=10&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1730,12 +1730,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>P086</t>
+          <t>P080</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-868064080-salsa-naranja-chipotle-38-lt-_JM#position=49&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-874583274-salsa-tamarindo-para-alitas-38-l-al-mejor-precio-_JM#position=22&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1778,12 +1778,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>P078</t>
+          <t>P080</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-814451280-salsa-teriyaki-38-lts-para-alitas-al-mejor-precio-_JM#position=1&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://www.mercadolibre.com.mx/mr-wings-tamarindo-en-galon-38l/p/MLM16595091?pdp_filters=seller_id:206710930#searchVariation=MLM16595091&amp;position=2&amp;search_layout=stack&amp;type=product&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1826,12 +1826,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>P075</t>
+          <t>P081</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-825295407-salsa-pina-hot-para-alitas-38-l-al-mejor-precio-_JM#position=4&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-756571010-salsa-picante-bbq-barbecue-habanero-para-alitas-38-l-_JM#position=27&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1874,12 +1874,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>P079</t>
+          <t>P081</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-788982442-salsa-bbq-barbecue-38l-para-alitas-mr-wings-al-mejor-precio-_JM#position=5&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-875617343-salsa-bbq-habanero-para-para-alitas-38-l-al-mejor-precio-_JM#position=47&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1922,12 +1922,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>P093</t>
+          <t>P082</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-799001903-salsa-lemon-pepper-para-alitas-1-galon-_JM#position=6&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-755930111-sazonador-lemon-pepper-hot-polvo-bote-800g-al-mejor-precio-_JM#position=30&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1970,12 +1970,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-825433680-paquete-de-4-salsas-para-alitas-_JM#position=9&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>P083</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-825433680-paquete-de-4-salsas-para-alitas-_JM#position=9&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-755921589-salsa-extra-hot-38l-salsa-extra-picante-para-alitas-_JM#position=26&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2018,12 +2018,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-819533373-16-muestras-de-salsas-_JM#position=11&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>P083</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-819533373-16-muestras-de-salsas-_JM#position=11&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-923131178-salsa-extra-hot-38l-salsa-extra-picante-para-alitas-_JM#position=38&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2066,12 +2066,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>P069</t>
+          <t>P084</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-825377787-salsa-bufalo-para-alitas-38-l-al-mejor-precio-_JM#position=12&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-756567694-sazonador-fuego-en-polvo-bote-800g-al-mejor-precio-_JM#position=33&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2114,12 +2114,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>P101</t>
+          <t>P085</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-865372434-salsa-ajo-parmesano-para-alitas-38-l-_JM#position=17&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-756567270-salsa-picante-cajun-para-alitas-38-l-al-mejor-precio-_JM#position=28&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2162,12 +2162,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>P071</t>
+          <t>P085</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-756582654-salsa-picante-original-h-para-alitas-38-l-al-mejor-precio-_JM#position=19&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-875618411-salsa-cajun-para-alitas-378-l-al-mejor-precio-_JM#position=4&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2210,12 +2210,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>P080</t>
+          <t>P086</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-874583274-salsa-tamarindo-para-alitas-38-l-al-mejor-precio-_JM#position=22&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-756582084-salsa-naranja-chipotle-para-alitas-38-l-al-mejor-precio-_JM#position=21&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2258,12 +2258,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>P076</t>
+          <t>P086</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-868471591-salsa-bbq-chipotle-_JM#position=25&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-868064080-salsa-naranja-chipotle-38-lt-_JM#position=49&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2306,12 +2306,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-874621959-caja-de-4-salsas-sabor-mango-habanero-para-alitas-38-l-_JM#position=28&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>P088</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-874621959-caja-de-4-salsas-sabor-mango-habanero-para-alitas-38-l-_JM#position=28&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-755917478-sazonador-chedar-en-polvo-800g-_JM#position=44&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2354,12 +2354,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-831255712-paquete-de-8-salsas-para-alitas-de-42kg-cada-_JM#position=30&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>P089</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-831255712-paquete-de-8-salsas-para-alitas-de-42kg-cada-_JM#position=30&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-756586580-sazonador-lemon-pepper-en-polvo-bote-800g-al-mejor-precio-_JM#position=16&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2402,12 +2402,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>P074</t>
+          <t>P093</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-874460232-salsa-para-alitas-crema-de-habanero-38lts-_JM#position=34&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-756586369-salsa-lemon-pepper-para-alitas-38-l-al-mejor-precio-_JM#position=7&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2450,12 +2450,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>P077</t>
+          <t>P093</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-874397634-salsa-mango-habanero-42kg-para-alitas-_JM#position=37&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-799001903-salsa-lemon-pepper-para-alitas-1-galon-_JM#position=6&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2498,12 +2498,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>P083</t>
+          <t>P101</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-923131178-salsa-extra-hot-38l-salsa-extra-picante-para-alitas-_JM#position=38&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-755933726-salsa-ajo-parmesano-38-lts-para-alitas-al-mejor-precio-_JM#position=8&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2546,12 +2546,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>P-0155</t>
+          <t>P101</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-893622220-salsa-sabor-mezcal-38lt-_JM#position=43&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-865372434-salsa-ajo-parmesano-para-alitas-38-l-_JM#position=17&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2594,12 +2594,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>P088</t>
+          <t>P137</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-755917478-sazonador-chedar-en-polvo-800g-_JM#position=44&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-848013478-salsa-de-guacamole-para-alitas-38-l-al-mejor-precio-_JM#position=32&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2642,17 +2642,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>P081</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-1307751214-sazonador-saborizante-tipo-takis-fuego-en-polvo-500gr-deliux-_JM</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-875617343-salsa-bbq-habanero-para-para-alitas-38-l-al-mejor-precio-_JM#position=47&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-1307751214-sazonador-saborizante-tipo-takis-fuego-en-polvo-500gr-deliux-_JM</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Mr Wings</t>
+          <t>Sazonador</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -2690,17 +2690,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>P085</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-629294328-aderezo-ranch-alitas-1-pieza-5-l-ensalada-restaurantes-_JM#position=19&amp;search_layout=stack&amp;type=pad&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68&amp;is_advertising=true&amp;ad_domain=VQCATCORE_LST&amp;ad_position=19&amp;ad_click_id=MDI5YmYzNDAtYTc5Ny00Y2RkLWE4OTUtYzIxZGYyOWQxMDgw</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-875618411-salsa-cajun-para-alitas-378-l-al-mejor-precio-_JM#position=4&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-629294328-aderezo-ranch-alitas-1-pieza-5-l-ensalada-restaurantes-_JM#position=19&amp;search_layout=stack&amp;type=pad&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68&amp;is_advertising=true&amp;ad_domain=VQCATCORE_LST&amp;ad_position=19&amp;ad_click_id=MDI5YmYzNDAtYTc5Ny00Y2RkLWE4OTUtYzIxZGYyOWQxMDgw</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Mr Wings</t>
+          <t>Inigualable</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
@@ -2738,17 +2738,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>P082</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-634347724-inigualable-salsa-alitas-bbq-clasica-1-garrafa-378-l-_JM#position=25&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-755930111-sazonador-lemon-pepper-hot-polvo-bote-800g-al-mejor-precio-_JM#position=30&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-634347724-inigualable-salsa-alitas-bbq-clasica-1-garrafa-378-l-_JM#position=25&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Mr Wings</t>
+          <t>Inigualable</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
@@ -2786,17 +2786,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>P077</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-634348864-inigualable-salsa-alitas-bbq-chipotle-1-garrafa-378-l-_JM#position=39&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904247331-salsa-para-alitas-mango-habanero-23-kg-_JM#position=31&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-634348864-inigualable-salsa-alitas-bbq-chipotle-1-garrafa-378-l-_JM#position=39&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Mr Wings</t>
+          <t>Inigualable</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
@@ -2834,17 +2834,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904246554-salsa-bbq-zafran-4-kg-_JM#position=30&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-634348989-inigualable-salsa-alitas-buf-wings-1-garrafa-378-l-red-hot-_JM#position=44&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904246554-salsa-bbq-zafran-4-kg-_JM#position=30&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-634348989-inigualable-salsa-alitas-buf-wings-1-garrafa-378-l-red-hot-_JM#position=44&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>Inigualable</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
@@ -2882,17 +2882,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-905157597-salsa-bbq-chile-ancho-22kg-custom-culinary-zafran-_JM#position=29&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-660174259-salsa-de-soya-5-litros-dragon-rojo-china-japonesa-sushi-_JM</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-905157597-salsa-bbq-chile-ancho-22kg-custom-culinary-zafran-_JM#position=29&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-660174259-salsa-de-soya-5-litros-dragon-rojo-china-japonesa-sushi-_JM</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>Inigualable</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
@@ -2930,17 +2930,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904274629-salsa-jugo-sazonador-41-kg-custom-culinary-zafran-_JM#position=34&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-726165420-extracto-de-stevia-liquida-natural-no-amarga-_JM</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904274629-salsa-jugo-sazonador-41-kg-custom-culinary-zafran-_JM#position=34&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-726165420-extracto-de-stevia-liquida-natural-no-amarga-_JM</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>Sin azúcar</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
@@ -2978,17 +2978,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-905177330-salsa-tipo-inglesa-1-lt-zafran-custom-culinary-_JM#position=36&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-728716313-eritritol-1-kg-jungbunzlauer-100-natural-_JM</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-905177330-salsa-tipo-inglesa-1-lt-zafran-custom-culinary-_JM#position=36&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-728716313-eritritol-1-kg-jungbunzlauer-100-natural-_JM</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>Sin azúcar</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
@@ -3026,17 +3026,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904257486-salsa-para-alitas-375-kg-zafran-custom-culinary-_JM#position=38&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-742060144-acido-citrico-1-kg-_JM</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904257486-salsa-para-alitas-375-kg-zafran-custom-culinary-_JM#position=38&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-742060144-acido-citrico-1-kg-_JM</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>Ingredientes</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
@@ -3074,17 +3074,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-905167004-salsa-extra-hot-extra-picante-2kg-custom-culinary-zafran-_JM#position=39&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-760483638-sriracha-salsa-picante-793g-original-_JM#position=3&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-905167004-salsa-extra-hot-extra-picante-2kg-custom-culinary-zafran-_JM#position=39&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-760483638-sriracha-salsa-picante-793g-original-_JM#position=3&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>Sriracha</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
@@ -3122,17 +3122,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-905175670-salsa-tipo-inglesa-21-kg-zafran-custom-culinary-_JM#position=40&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-761995023-sriracha-salsa-picante-huy-fong-793g-_JM#position=13&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-905175670-salsa-tipo-inglesa-21-kg-zafran-custom-culinary-_JM#position=40&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-761995023-sriracha-salsa-picante-huy-fong-793g-_JM#position=13&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>Sriracha</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
@@ -3170,17 +3170,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-910390691-salsa-bbq-cubeta-de-18-kilos-mayoreo-para-alitas-o-costillas-_JM#position=42&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-777978939-tofu-extra-firme-12-piezas-349g-libre-de-gluten-_JM</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-910390691-salsa-bbq-cubeta-de-18-kilos-mayoreo-para-alitas-o-costillas-_JM#position=42&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-777978939-tofu-extra-firme-12-piezas-349g-libre-de-gluten-_JM</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>Vegano</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
@@ -3218,17 +3218,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-905150986-aderezo-blue-cheese-36-kg-custom-culinary-zafran-_JM#position=43&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-781752942-crema-de-cacahuate-oaxaqueno-sin-azucar-100-natural-220g-_JM</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-905150986-aderezo-blue-cheese-36-kg-custom-culinary-zafran-_JM#position=43&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-781752942-crema-de-cacahuate-oaxaqueno-sin-azucar-100-natural-220g-_JM</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>Crema de cacahate</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
@@ -3266,17 +3266,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904263739-jugo-sazonador-tipo-maggi-22kg-custom-culinary-zafran-_JM#position=44&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-790447226-caja-de-salsa-sriracha-con-12-piezas-de-793-g-_JM#position=48&amp;search_layout=stack&amp;type=item&amp;tracking_id=bedcf8aa-55cc-4adb-bf03-23858a282b78</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904263739-jugo-sazonador-tipo-maggi-22kg-custom-culinary-zafran-_JM#position=44&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-790447226-caja-de-salsa-sriracha-con-12-piezas-de-793-g-_JM#position=48&amp;search_layout=stack&amp;type=item&amp;tracking_id=bedcf8aa-55cc-4adb-bf03-23858a282b78</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>Sriracha</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
@@ -3314,17 +3314,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904255161-5-salsas-zafran-custom-c-bbq-alitasbbq-hot-mango-lemon-_JM#position=7&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-800668712-aderezo-blue-cheese-la-duena-2lt-innigualable-sabor-_JM#position=21&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904255161-5-salsas-zafran-custom-c-bbq-alitasbbq-hot-mango-lemon-_JM#position=7&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-800668712-aderezo-blue-cheese-la-duena-2lt-innigualable-sabor-_JM#position=21&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>La Duena</t>
         </is>
       </c>
       <c r="D58" t="inlineStr"/>
@@ -3362,17 +3362,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904257210-salsa-hot-bbq-24-kg-zafran-custom-culinary-_JM#position=8&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-819533373-16-muestras-de-salsas-_JM#position=11&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-904257210-salsa-hot-bbq-24-kg-zafran-custom-culinary-_JM#position=8&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-819533373-16-muestras-de-salsas-_JM#position=11&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Custom Culinary</t>
+          <t>Mr Wings</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
@@ -3410,17 +3410,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-800668712-aderezo-blue-cheese-la-duena-2lt-innigualable-sabor-_JM#position=21&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-825433680-paquete-de-4-salsas-para-alitas-_JM#position=9&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-800668712-aderezo-blue-cheese-la-duena-2lt-innigualable-sabor-_JM#position=21&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-825433680-paquete-de-4-salsas-para-alitas-_JM#position=9&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>La Duena</t>
+          <t>Mr Wings</t>
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
@@ -3458,17 +3458,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-910391598-salsa-picante-para-alitas-18kg-original-mayoreo-_JM#position=19&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-831255712-paquete-de-8-salsas-para-alitas-de-42kg-cada-_JM#position=30&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-910391598-salsa-picante-para-alitas-18kg-original-mayoreo-_JM#position=19&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-831255712-paquete-de-8-salsas-para-alitas-de-42kg-cada-_JM#position=30&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Inigualable</t>
+          <t>Mr Wings</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
@@ -3506,17 +3506,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-903136780-aderezo-ranch-38lt-_JM#position=48&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-849872386-salsa-abal-para-alitas-costillas-cocinar-bbq-barbecue-4kg-_JM#position=17&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-903136780-aderezo-ranch-38lt-_JM#position=48&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-849872386-salsa-abal-para-alitas-costillas-cocinar-bbq-barbecue-4kg-_JM#position=17&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Inigualable</t>
+          <t>Abal</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
@@ -3554,17 +3554,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-760483638-sriracha-salsa-picante-793g-original-_JM#position=3&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-861868855-mix-de-sales-para-preparar-electrolitos-sin-azucar-low-carb-_JM</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-760483638-sriracha-salsa-picante-793g-original-_JM#position=3&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-861868855-mix-de-sales-para-preparar-electrolitos-sin-azucar-low-carb-_JM</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Sriracha</t>
+          <t>Keto</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
@@ -3602,17 +3602,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-761995023-sriracha-salsa-picante-huy-fong-793g-_JM#position=13&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-874621959-caja-de-4-salsas-sabor-mango-habanero-para-alitas-38-l-_JM#position=28&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-761995023-sriracha-salsa-picante-huy-fong-793g-_JM#position=13&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-874621959-caja-de-4-salsas-sabor-mango-habanero-para-alitas-38-l-_JM#position=28&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Sriracha</t>
+          <t>Mr Wings</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
@@ -3650,17 +3650,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-849872386-salsa-abal-para-alitas-costillas-cocinar-bbq-barbecue-4kg-_JM#position=17&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-891990008-kefir-coco-4-pack-_JM</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-849872386-salsa-abal-para-alitas-costillas-cocinar-bbq-barbecue-4kg-_JM#position=17&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-891990008-kefir-coco-4-pack-_JM</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Abal</t>
+          <t>Vegano</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
@@ -3698,17 +3698,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>https://www.mercadolibre.com.mx/salsa-abal-para-alitas-costillas-cocinar-bbq-barbecue-4kg/p/MLM19629577</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-903136780-aderezo-ranch-38lt-_JM#position=48&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://www.mercadolibre.com.mx/salsa-abal-para-alitas-costillas-cocinar-bbq-barbecue-4kg/p/MLM19629577</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-903136780-aderezo-ranch-38lt-_JM#position=48&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Abal</t>
+          <t>Inigualable</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
@@ -3746,17 +3746,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-629294328-aderezo-ranch-alitas-1-pieza-5-l-ensalada-restaurantes-_JM#position=19&amp;search_layout=stack&amp;type=pad&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68&amp;is_advertising=true&amp;ad_domain=VQCATCORE_LST&amp;ad_position=19&amp;ad_click_id=MDI5YmYzNDAtYTc5Ny00Y2RkLWE4OTUtYzIxZGYyOWQxMDgw</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904246554-salsa-bbq-zafran-4-kg-_JM#position=30&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-629294328-aderezo-ranch-alitas-1-pieza-5-l-ensalada-restaurantes-_JM#position=19&amp;search_layout=stack&amp;type=pad&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68&amp;is_advertising=true&amp;ad_domain=VQCATCORE_LST&amp;ad_position=19&amp;ad_click_id=MDI5YmYzNDAtYTc5Ny00Y2RkLWE4OTUtYzIxZGYyOWQxMDgw</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904246554-salsa-bbq-zafran-4-kg-_JM#position=30&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Inigualable</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
@@ -3794,17 +3794,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-634347724-inigualable-salsa-alitas-bbq-clasica-1-garrafa-378-l-_JM#position=25&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904255161-5-salsas-zafran-custom-c-bbq-alitasbbq-hot-mango-lemon-_JM#position=7&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-634347724-inigualable-salsa-alitas-bbq-clasica-1-garrafa-378-l-_JM#position=25&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904255161-5-salsas-zafran-custom-c-bbq-alitasbbq-hot-mango-lemon-_JM#position=7&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Inigualable</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
@@ -3842,17 +3842,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-634348864-inigualable-salsa-alitas-bbq-chipotle-1-garrafa-378-l-_JM#position=39&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904257210-salsa-hot-bbq-24-kg-zafran-custom-culinary-_JM#position=8&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-634348864-inigualable-salsa-alitas-bbq-chipotle-1-garrafa-378-l-_JM#position=39&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904257210-salsa-hot-bbq-24-kg-zafran-custom-culinary-_JM#position=8&amp;search_layout=stack&amp;type=item&amp;tracking_id=3817b8b0-4bd8-40d1-8dd0-1f1e8548b734</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Inigualable</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D69" t="inlineStr"/>
@@ -3890,17 +3890,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-634348989-inigualable-salsa-alitas-buf-wings-1-garrafa-378-l-red-hot-_JM#position=44&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904257486-salsa-para-alitas-375-kg-zafran-custom-culinary-_JM#position=38&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-634348989-inigualable-salsa-alitas-buf-wings-1-garrafa-378-l-red-hot-_JM#position=44&amp;search_layout=stack&amp;type=item&amp;tracking_id=14462c17-0a51-4a5d-9b15-182028b4dd68</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904257486-salsa-para-alitas-375-kg-zafran-custom-culinary-_JM#position=38&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Inigualable</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
@@ -3938,17 +3938,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-790447226-caja-de-salsa-sriracha-con-12-piezas-de-793-g-_JM#position=48&amp;search_layout=stack&amp;type=item&amp;tracking_id=bedcf8aa-55cc-4adb-bf03-23858a282b78</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904263739-jugo-sazonador-tipo-maggi-22kg-custom-culinary-zafran-_JM#position=44&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-790447226-caja-de-salsa-sriracha-con-12-piezas-de-793-g-_JM#position=48&amp;search_layout=stack&amp;type=item&amp;tracking_id=bedcf8aa-55cc-4adb-bf03-23858a282b78</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904263739-jugo-sazonador-tipo-maggi-22kg-custom-culinary-zafran-_JM#position=44&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Sriracha</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D71" t="inlineStr"/>
@@ -3986,17 +3986,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>https://www.mercadolibre.com.mx/ketchup-heinz-sin-azucar-anadida-pet-369g/p/MLM18974685</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904274629-salsa-jugo-sazonador-41-kg-custom-culinary-zafran-_JM#position=34&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://www.mercadolibre.com.mx/ketchup-heinz-sin-azucar-anadida-pet-369g/p/MLM18974685</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-904274629-salsa-jugo-sazonador-41-kg-custom-culinary-zafran-_JM#position=34&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Sin azúcar</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
@@ -4034,17 +4034,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-660174259-salsa-de-soya-5-litros-dragon-rojo-china-japonesa-sushi-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-905150986-aderezo-blue-cheese-36-kg-custom-culinary-zafran-_JM#position=43&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-660174259-salsa-de-soya-5-litros-dragon-rojo-china-japonesa-sushi-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-905150986-aderezo-blue-cheese-36-kg-custom-culinary-zafran-_JM#position=43&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Inigualable</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
@@ -4082,17 +4082,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-1307751214-sazonador-saborizante-tipo-takis-fuego-en-polvo-500gr-deliux-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-905157597-salsa-bbq-chile-ancho-22kg-custom-culinary-zafran-_JM#position=29&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-1307751214-sazonador-saborizante-tipo-takis-fuego-en-polvo-500gr-deliux-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-905157597-salsa-bbq-chile-ancho-22kg-custom-culinary-zafran-_JM#position=29&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Sazonador</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D74" t="inlineStr"/>
@@ -4130,17 +4130,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-950161881-crema-de-cacahuate-cremosa-organica-kirkland-7938gr-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-905167004-salsa-extra-hot-extra-picante-2kg-custom-culinary-zafran-_JM#position=39&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-950161881-crema-de-cacahuate-cremosa-organica-kirkland-7938gr-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-905167004-salsa-extra-hot-extra-picante-2kg-custom-culinary-zafran-_JM#position=39&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Crema de cacahate</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D75" t="inlineStr"/>
@@ -4178,17 +4178,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-777978939-tofu-extra-firme-12-piezas-349g-libre-de-gluten-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-905175670-salsa-tipo-inglesa-21-kg-zafran-custom-culinary-_JM#position=40&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-777978939-tofu-extra-firme-12-piezas-349g-libre-de-gluten-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-905175670-salsa-tipo-inglesa-21-kg-zafran-custom-culinary-_JM#position=40&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Vegano</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D76" t="inlineStr"/>
@@ -4226,17 +4226,17 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-861868855-mix-de-sales-para-preparar-electrolitos-sin-azucar-low-carb-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-905177330-salsa-tipo-inglesa-1-lt-zafran-custom-culinary-_JM#position=36&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-861868855-mix-de-sales-para-preparar-electrolitos-sin-azucar-low-carb-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-905177330-salsa-tipo-inglesa-1-lt-zafran-custom-culinary-_JM#position=36&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Keto</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
@@ -4274,17 +4274,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-891990008-kefir-coco-4-pack-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-910390691-salsa-bbq-cubeta-de-18-kilos-mayoreo-para-alitas-o-costillas-_JM#position=42&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-891990008-kefir-coco-4-pack-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-910390691-salsa-bbq-cubeta-de-18-kilos-mayoreo-para-alitas-o-costillas-_JM#position=42&amp;search_layout=stack&amp;type=item&amp;tracking_id=07900876-48a9-42ef-b9d6-fe34affd9c03</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Vegano</t>
+          <t>Custom Culinary</t>
         </is>
       </c>
       <c r="D78" t="inlineStr"/>
@@ -4322,17 +4322,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>https://www.mercadolibre.com.mx/edulcorante-the-functional-foods-fruta-del-monje-en-polvo-sin-gluten-bolsa-400g/p/MLM17518226</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-910391598-salsa-picante-para-alitas-18kg-original-mayoreo-_JM#position=19&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://www.mercadolibre.com.mx/edulcorante-the-functional-foods-fruta-del-monje-en-polvo-sin-gluten-bolsa-400g/p/MLM17518226</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-910391598-salsa-picante-para-alitas-18kg-original-mayoreo-_JM#position=19&amp;search_layout=stack&amp;type=item&amp;tracking_id=269eb207-0f3a-4491-8c18-84bd9ee56400</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Sin azúcar</t>
+          <t>Inigualable</t>
         </is>
       </c>
       <c r="D79" t="inlineStr"/>
@@ -4370,17 +4370,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-726165420-extracto-de-stevia-liquida-natural-no-amarga-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-950161881-crema-de-cacahuate-cremosa-organica-kirkland-7938gr-_JM</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-726165420-extracto-de-stevia-liquida-natural-no-amarga-_JM</t>
+          <t>https://articulo.mercadolibre.com.mx/MLM-950161881-crema-de-cacahuate-cremosa-organica-kirkland-7938gr-_JM</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Sin azúcar</t>
+          <t>Crema de cacahate</t>
         </is>
       </c>
       <c r="D80" t="inlineStr"/>
@@ -4418,12 +4418,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-728716313-eritritol-1-kg-jungbunzlauer-100-natural-_JM</t>
+          <t>https://www.mercadolibre.com.mx/edulcorante-the-functional-foods-fruta-del-monje-en-polvo-sin-gluten-bolsa-400g/p/MLM17518226</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-728716313-eritritol-1-kg-jungbunzlauer-100-natural-_JM</t>
+          <t>https://www.mercadolibre.com.mx/edulcorante-the-functional-foods-fruta-del-monje-en-polvo-sin-gluten-bolsa-400g/p/MLM17518226</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -4466,17 +4466,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-742060144-acido-citrico-1-kg-_JM</t>
+          <t>https://www.mercadolibre.com.mx/ketchup-heinz-sin-azucar-anadida-pet-369g/p/MLM18974685</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-742060144-acido-citrico-1-kg-_JM</t>
+          <t>https://www.mercadolibre.com.mx/ketchup-heinz-sin-azucar-anadida-pet-369g/p/MLM18974685</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Ingredientes</t>
+          <t>Sin azúcar</t>
         </is>
       </c>
       <c r="D82" t="inlineStr"/>
@@ -4514,17 +4514,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-781752942-crema-de-cacahuate-oaxaqueno-sin-azucar-100-natural-220g-_JM</t>
+          <t>https://www.mercadolibre.com.mx/mr-wings-ajo-parmesano-en-galon-38l/p/MLM16595103</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://articulo.mercadolibre.com.mx/MLM-781752942-crema-de-cacahuate-oaxaqueno-sin-azucar-100-natural-220g-_JM</t>
+          <t>https://www.mercadolibre.com.mx/mr-wings-ajo-parmesano-en-galon-38l/p/MLM16595103</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Crema de cacahate</t>
+          <t>Mr Wings</t>
         </is>
       </c>
       <c r="D83" t="inlineStr"/>
@@ -4562,12 +4562,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>https://www.mercadolibre.com.mx/mr-wings-ajo-parmesano-en-galon-38l/p/MLM16595103</t>
+          <t>https://www.mercadolibre.com.mx/mr-wings-honey-mustard-en-galon-38l/p/MLM16595113</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://www.mercadolibre.com.mx/mr-wings-ajo-parmesano-en-galon-38l/p/MLM16595103</t>
+          <t>https://www.mercadolibre.com.mx/mr-wings-honey-mustard-en-galon-38l/p/MLM16595113</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -4610,17 +4610,17 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>https://www.mercadolibre.com.mx/mr-wings-honey-mustard-en-galon-38l/p/MLM16595113</t>
+          <t>https://www.mercadolibre.com.mx/salsa-abal-para-alitas-costillas-cocinar-bbq-barbecue-4kg/p/MLM19629577</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://www.mercadolibre.com.mx/mr-wings-honey-mustard-en-galon-38l/p/MLM16595113</t>
+          <t>https://www.mercadolibre.com.mx/salsa-abal-para-alitas-costillas-cocinar-bbq-barbecue-4kg/p/MLM19629577</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Mr Wings</t>
+          <t>Abal</t>
         </is>
       </c>
       <c r="D85" t="inlineStr"/>

</xml_diff>